<commit_message>
Avoid NPE when cell for indicator is null
</commit_message>
<xml_diff>
--- a/samples/Lines.xlsx
+++ b/samples/Lines.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -86,6 +86,21 @@
   </si>
   <si>
     <t xml:space="preserve">true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marie Curie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Otherland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rue de la Chanson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paris</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Madame Curie</t>
   </si>
 </sst>
 </file>
@@ -254,7 +269,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
@@ -262,12 +277,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.8178137651822"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.81781376518219"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.3522267206478"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.4615384615385"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -401,6 +416,26 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
+    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>43828</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Add a Date to the samples to see how it is formatted currently
</commit_message>
<xml_diff>
--- a/samples/Lines.xlsx
+++ b/samples/Lines.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t xml:space="preserve">Include</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date</t>
   </si>
   <si>
     <t xml:space="preserve">Ginger Rogers</t>
@@ -107,8 +110,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="D/\ MMMM\ YYYY"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -183,12 +187,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -272,168 +284,181 @@
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0323886639676"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.81781376518219"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.4615384615385"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="19.3603238866397"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="n">
         <v>10010</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="1" t="n">
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
+      <c r="H2" s="3" t="n">
+        <v>42370</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="n">
         <v>10014</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
+      <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="3" t="n">
+        <v>43092</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="C4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2" t="n">
         <v>1040</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
+      <c r="G4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="3" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>43828</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>77514</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix handling of special characters, especially ampersand "&"
Requires escaping for XML
New dependency commons-text for StringEscapeUtils
Add tests
</commit_message>
<xml_diff>
--- a/samples/Lines.xlsx
+++ b/samples/Lines.xlsx
@@ -5,10 +5,10 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -104,6 +104,24 @@
   </si>
   <si>
     <t xml:space="preserve">Madame Curie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some special char &amp;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">and others &lt; and &gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Let's try,Another!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W?ß\</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!§$%&amp;/()=?][{}],</t>
   </si>
 </sst>
 </file>
@@ -112,9 +130,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="D/\ MMMM\ YYYY"/>
+    <numFmt numFmtId="165" formatCode="d/\ mmmm\ yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -144,6 +162,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -187,31 +211,51 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -276,195 +320,321 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0323886639676"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.81781376518219"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.5668016194332"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="19.3603238866397"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="19.36"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="1" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="3" t="n">
         <v>10010</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="H2" s="3" t="n">
+      <c r="H2" s="4" t="n">
         <v>42370</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="3" t="n">
         <v>10014</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="3" t="n">
+      <c r="G3" s="3"/>
+      <c r="H3" s="4" t="n">
         <v>43092</v>
       </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="3" t="n">
         <v>1040</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="3" t="n">
+      <c r="H4" s="4" t="n">
         <v>25934</v>
       </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>43828</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="1" t="n">
+      <c r="H5" s="2" t="n">
         <v>77514</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>